<commit_message>
Implementation design of new sync objects
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.R2.xlsx
+++ b/RTuinOS/doc/effort.R2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Concept of new sync objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation design of new sync objects </t>
   </si>
 </sst>
 </file>
@@ -850,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -912,6 +915,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>41426</v>
+      </c>
+      <c r="B5">
+        <v>0.75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update of manual with respect to mutex and semaphore. Introduction and outlook still need to be done besides a general review
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.R2.xlsx
+++ b/RTuinOS/doc/effort.R2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -37,7 +37,13 @@
     <t>Concept of new sync objects</t>
   </si>
   <si>
-    <t xml:space="preserve">Implementation design of new sync objects </t>
+    <t xml:space="preserve">Design of implementation new sync objects </t>
+  </si>
+  <si>
+    <t>Implementation of mutexes</t>
+  </si>
+  <si>
+    <t>Update Manual</t>
   </si>
 </sst>
 </file>
@@ -853,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -926,6 +932,39 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>41430</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>41431</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>41432</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementation of mutexes done. No single test has been run yet. It has been proven (by samples only), that the existing test cases are still running
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.R2.xlsx
+++ b/RTuinOS/doc/effort.R2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Update Manual</t>
+  </si>
+  <si>
+    <t>Implementation of mutexes: Basically done. No test case implemented yet, no testing done yet</t>
   </si>
 </sst>
 </file>
@@ -859,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -959,10 +962,35 @@
         <v>41432</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>41432</v>
+      </c>
+      <c r="B9">
+        <v>2.25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>41435</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First test case for mutex implementation made. tc11 is completed and succeeds
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.R2.xlsx
+++ b/RTuinOS/doc/effort.R2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Implementation of mutexes: Basically done. No test case implemented yet, no testing done yet</t>
+  </si>
+  <si>
+    <t>Implementation of tc11_mutex</t>
   </si>
 </sst>
 </file>
@@ -862,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -993,6 +996,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>41436</v>
+      </c>
+      <c r="B11">
+        <v>1.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Makefile: Support of floating point library versions for formatted output (printf). This version of the libraries becomes the new default.   rtos.c: Implementation of semaphores done, but only very preliminary tests have been run yet, by using a semaphore instead of the mutex in a copy of tc11.   tc12: Starting point for a semaphore test case, implementing a data queue. Not yet finished. This revision of the test case is runnable and demonstrates how to use printf for communication via COM
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.R2.xlsx
+++ b/RTuinOS/doc/effort.R2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Implementation of tc11_mutex</t>
+  </si>
+  <si>
+    <t>Implementation of semaphores and first, very preliminary but successfuls tests</t>
   </si>
 </sst>
 </file>
@@ -865,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1007,6 +1010,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>41439</v>
+      </c>
+      <c r="B12">
+        <v>1.5</v>
+      </c>
+      <c r="C12">
+        <v>2.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementation of test case 12: Most code is there and the application is more or less running but several problems have already been found. Particularly with the handling of initial resume conditions for new tasks at RTuinOS start up. Furthermore, we still have an unexpected timing of the producer task and the CPU is shown as 100%, which is unreasonable
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.R2.xlsx
+++ b/RTuinOS/doc/effort.R2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Implementation of semaphores and first, very preliminary but successfuls tests</t>
+  </si>
+  <si>
+    <t>Implementation tc12</t>
   </si>
 </sst>
 </file>
@@ -868,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1024,6 +1027,28 @@
         <v>12</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>41440</v>
+      </c>
+      <c r="B13">
+        <v>2.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>41442</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix, RTuinOS: Handling of repeated posts of the same semaphore was bad if the task stayed suspended after the first post.   Test case 12: completely implemented and successful   Makefile: Default is now not to link against the printf library with flaoting point support. Instead, a remark will be entered in all test cases which require it (this is done in tc12)
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.R2.xlsx
+++ b/RTuinOS/doc/effort.R2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -871,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1049,6 +1049,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>41443</v>
+      </c>
+      <c r="B15">
+        <v>1.5</v>
+      </c>
+      <c r="C15">
+        <v>2.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
gsl_systemLoad: Becomes a true part of RTuinOS (moved to other, common folder).   New test case tc13: Concept and part of implementation done.   Makefile: Code and data size redirected into the map file.   Documentation of effort merged with file of RTuinOS 0.9
</commit_message>
<xml_diff>
--- a/RTuinOS/doc/effort.R2.xlsx
+++ b/RTuinOS/doc/effort.R2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -55,7 +55,10 @@
     <t>Implementation of semaphores and first, very preliminary but successfuls tests</t>
   </si>
   <si>
-    <t>Implementation tc12</t>
+    <t>Implementation tc12_queue</t>
+  </si>
+  <si>
+    <t>Design and implementation tc13_eventStates</t>
   </si>
 </sst>
 </file>
@@ -871,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1054,13 +1057,27 @@
         <v>41443</v>
       </c>
       <c r="B15">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>41444</v>
+      </c>
+      <c r="B16">
+        <v>1.5</v>
+      </c>
+      <c r="C16">
+        <v>2.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>